<commit_message>
Refining document and inspection
</commit_message>
<xml_diff>
--- a/Working directory/CI/Inspection.xlsx
+++ b/Working directory/CI/Inspection.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Documents\SE2 Project\swe2-project\Working directory\Inspection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andre\Documents\SE2 Project\swe2-project\Working directory\CI\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
   <si>
     <t>Line</t>
   </si>
@@ -50,12 +50,6 @@
     <t>constant with lowecase name</t>
   </si>
   <si>
-    <t>3 spaces for indention instead of 4 like the rest of document</t>
-  </si>
-  <si>
-    <t>statement not aligned</t>
-  </si>
-  <si>
     <t>empty case block without break or return</t>
   </si>
   <si>
@@ -65,15 +59,6 @@
     <t>_getContextForInstance</t>
   </si>
   <si>
-    <t>_constructEJBContextImpl</t>
-  </si>
-  <si>
-    <t>_constructEJBInstance</t>
-  </si>
-  <si>
-    <t>createBeanInstance</t>
-  </si>
-  <si>
     <t>destroyExtendedEMsForContext</t>
   </si>
   <si>
@@ -86,20 +71,65 @@
     <t>doVersionCheck</t>
   </si>
   <si>
-    <t>useless variable (constant)</t>
-  </si>
-  <si>
     <t>useless paramether (sessionKey) used only for log</t>
   </si>
   <si>
     <t>string concat can be avoided</t>
+  </si>
+  <si>
+    <t>method name pattern should be  [a-z][a-z0-9][a-zA-Z0-9_]*</t>
+  </si>
+  <si>
+    <t>_getContext</t>
+  </si>
+  <si>
+    <t>Abbreviation in name must contain no more than one capital letter</t>
+  </si>
+  <si>
+    <t>useless blank line</t>
+  </si>
+  <si>
+    <t>wrong indentation and duplicated '+'</t>
+  </si>
+  <si>
+    <t>Comment not explain adequately the method functions</t>
+  </si>
+  <si>
+    <t>Duplication Code lines: 1621, 1677, 1696. Can be avoided with a proper method</t>
+  </si>
+  <si>
+    <t>instead using paramether SessionContextImpl use List of PhysicalEntityManagerWrapper</t>
+  </si>
+  <si>
+    <t>commented line of code</t>
+  </si>
+  <si>
+    <t>incorrect output format</t>
+  </si>
+  <si>
+    <t>line can be less then 80 characters</t>
+  </si>
+  <si>
+    <t>static refence to a non static object</t>
+  </si>
+  <si>
+    <t>Useless parameters: SessionContextImpl, 'sessionKey' only for log</t>
+  </si>
+  <si>
+    <t>handelCurrentInvocation</t>
+  </si>
+  <si>
+    <t>splitted line not aligned</t>
+  </si>
+  <si>
+    <t>lines can be less then 80 characters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,7 +145,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFC000"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -141,10 +178,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -425,16 +463,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -449,7 +487,7 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -518,158 +556,320 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>732</v>
-      </c>
-      <c r="B8" s="2">
+    <row r="8" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1379</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1395</v>
+      </c>
+      <c r="B9" s="1">
+        <v>52</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>1454</v>
+      </c>
+      <c r="B10" s="2">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1462</v>
+      </c>
+      <c r="B11" s="2">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>1471</v>
+      </c>
+      <c r="B12" s="2">
+        <v>43</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>1476</v>
+      </c>
+      <c r="B13" s="2">
+        <v>19</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>1477</v>
+      </c>
+      <c r="B14" s="2">
+        <v>19</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>1476</v>
+      </c>
+      <c r="B15" s="2">
+        <v>54</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="2" t="s">
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>1480</v>
+      </c>
+      <c r="B16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>1754</v>
+      </c>
+      <c r="B17" s="3">
+        <v>29</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>1766</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1772</v>
+      </c>
+      <c r="B19" s="3">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>733</v>
-      </c>
-      <c r="B9" s="2">
+      <c r="C19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>1778</v>
+      </c>
+      <c r="B20" s="3">
+        <v>43</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>1605</v>
+      </c>
+      <c r="B21" s="2">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>738</v>
-      </c>
-      <c r="B10" s="2">
+      <c r="D21" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1676</v>
+      </c>
+      <c r="B22" s="2">
+        <v>6</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>1673</v>
+      </c>
+      <c r="B23" s="2">
+        <v>12</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>1645</v>
+      </c>
+      <c r="B24" s="2">
         <v>17</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>1652</v>
+      </c>
+      <c r="B25" s="2">
+        <v>17</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>1602</v>
+      </c>
+      <c r="B26" s="2">
+        <v>18</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>1605</v>
+      </c>
+      <c r="B27" s="2">
+        <v>27</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>1786</v>
+      </c>
+      <c r="B28" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>762</v>
-      </c>
-      <c r="B11" s="2">
+      <c r="C28" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>1786</v>
+      </c>
+      <c r="B29" s="1">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>1806</v>
+      </c>
+      <c r="B30" s="1">
         <v>17</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>763</v>
-      </c>
-      <c r="B12" s="2">
-        <v>17</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1395</v>
-      </c>
-      <c r="B13" s="1">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1462</v>
-      </c>
-      <c r="B14" s="1">
-        <v>56</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>1476</v>
-      </c>
-      <c r="B15" s="1">
-        <v>54</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>1754</v>
-      </c>
-      <c r="B16" s="1">
-        <v>29</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D16" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>1757</v>
-      </c>
-      <c r="B17" s="1">
-        <v>29</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>1778</v>
-      </c>
-      <c r="B18" s="1">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
+      <c r="C30" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D30" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>